<commit_message>
2016 ACS housing units added
</commit_message>
<xml_diff>
--- a/Data/Multifamily.xlsx
+++ b/Data/Multifamily.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taohe/Documents/GitHub/SLC-Housing-Dashboard/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taohe/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Multi-Family Listings" sheetId="1" r:id="rId1"/>
-    <sheet name="Research" sheetId="4" r:id="rId2"/>
+    <sheet name="ASC-Housing-2016" sheetId="5" r:id="rId2"/>
+    <sheet name="Research" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Multi-Family Listings'!$D$1:$D$219</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="639">
   <si>
     <t>Project Name</t>
   </si>
@@ -1879,10 +1880,79 @@
     <t>total</t>
   </si>
   <si>
-    <t>Market Units</t>
-  </si>
-  <si>
-    <t>Mixed Units</t>
+    <t>UNITS IN STRUCTURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Total housing units</t>
+  </si>
+  <si>
+    <t>83,759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      1-unit, detached</t>
+  </si>
+  <si>
+    <t>45.6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      1-unit, attached</t>
+  </si>
+  <si>
+    <t>3.0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      2 units</t>
+  </si>
+  <si>
+    <t>7.5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      3 or 4 units</t>
+  </si>
+  <si>
+    <t>7.4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      5 to 9 units</t>
+  </si>
+  <si>
+    <t>5.2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      10 to 19 units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      20 or more units</t>
+  </si>
+  <si>
+    <t>22.7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Mobile home</t>
+  </si>
+  <si>
+    <t>0.6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Boat, RV, van, etc.</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>single family toal</t>
+  </si>
+  <si>
+    <t>multifamily total</t>
+  </si>
+  <si>
+    <t>affordable percentage</t>
+  </si>
+  <si>
+    <t>Multifamily Units Total</t>
+  </si>
+  <si>
+    <t>Other Multifamily Units</t>
   </si>
 </sst>
 </file>
@@ -1893,7 +1963,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1948,8 +2018,13 @@
       <name val="BankGothic Lt BT"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="SansSerif"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1980,8 +2055,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2069,12 +2150,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2328,10 +2462,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2609,11 +2772,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P220"/>
+  <dimension ref="A1:P221"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K221" sqref="K221"/>
+      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J227" sqref="J227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2660,10 +2823,10 @@
         <v>6</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>614</v>
+        <v>638</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>615</v>
+        <v>637</v>
       </c>
       <c r="L1" s="37" t="s">
         <v>7</v>
@@ -9376,7 +9539,7 @@
         <v>127</v>
       </c>
       <c r="G194" s="2" t="str">
-        <f t="shared" ref="G194:G257" si="3">IF(H194-I194=H194,"Market",IF(H194-I194&gt;0,"Mixed","Affordable"))</f>
+        <f t="shared" ref="G194:G219" si="3">IF(H194-I194=H194,"Market",IF(H194-I194&gt;0,"Mixed","Affordable"))</f>
         <v>Affordable</v>
       </c>
       <c r="H194" s="9">
@@ -10278,21 +10441,26 @@
       <c r="A220" s="20" t="s">
         <v>613</v>
       </c>
-      <c r="H220" s="20">
-        <f>SUM(H2:H219)</f>
-        <v>18196</v>
-      </c>
       <c r="I220" s="20">
         <f>SUM(I2:I219)</f>
         <v>5993</v>
       </c>
-      <c r="J220" s="20">
-        <f>SUMIF(G2:G219, "Market", H2:H219)</f>
-        <v>10328</v>
-      </c>
-      <c r="K220" s="20">
-        <f>SUMIF(G2:G219, "Mixed", H2:H219)</f>
-        <v>3588</v>
+      <c r="K220" s="93">
+        <f>'ASC-Housing-2016'!I10</f>
+        <v>42636</v>
+      </c>
+    </row>
+    <row r="221" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A221" s="20" t="s">
+        <v>636</v>
+      </c>
+      <c r="I221" s="94">
+        <f>ROUND(I220/K220, 2)</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J221" s="94">
+        <f>1-I221</f>
+        <v>0.86</v>
       </c>
     </row>
   </sheetData>
@@ -10310,6 +10478,227 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="85" t="s">
+        <v>614</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="87" t="s">
+        <v>633</v>
+      </c>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="86"/>
+      <c r="H1" t="s">
+        <v>634</v>
+      </c>
+      <c r="I1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="85" t="s">
+        <v>615</v>
+      </c>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="91">
+        <v>83759</v>
+      </c>
+      <c r="E2" s="88"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="86" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="85" t="s">
+        <v>617</v>
+      </c>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="91">
+        <v>38157</v>
+      </c>
+      <c r="E3" s="88"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="86" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="85" t="s">
+        <v>619</v>
+      </c>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="91">
+        <v>2502</v>
+      </c>
+      <c r="E4" s="88"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="86" t="s">
+        <v>620</v>
+      </c>
+      <c r="H4" s="92">
+        <f>SUM(D3:D4)</f>
+        <v>40659</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="85" t="s">
+        <v>621</v>
+      </c>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="91">
+        <v>6312</v>
+      </c>
+      <c r="E5" s="88"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="86" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="85" t="s">
+        <v>623</v>
+      </c>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="91">
+        <v>6185</v>
+      </c>
+      <c r="E6" s="88"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="86" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="85" t="s">
+        <v>625</v>
+      </c>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="91">
+        <v>4347</v>
+      </c>
+      <c r="E7" s="88"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="86" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="85" t="s">
+        <v>627</v>
+      </c>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="91">
+        <v>6273</v>
+      </c>
+      <c r="E8" s="88"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="86" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="85" t="s">
+        <v>628</v>
+      </c>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="91">
+        <v>19004</v>
+      </c>
+      <c r="E9" s="88"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="86" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="85" t="s">
+        <v>630</v>
+      </c>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="90">
+        <v>515</v>
+      </c>
+      <c r="E10" s="88"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="86" t="s">
+        <v>631</v>
+      </c>
+      <c r="I10" s="92">
+        <f>SUM(D5:F10)</f>
+        <v>42636</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="85" t="s">
+        <v>632</v>
+      </c>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="90">
+        <v>464</v>
+      </c>
+      <c r="E11" s="88"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="86" t="s">
+        <v>631</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>

</xml_diff>